<commit_message>
added total brain volume
</commit_message>
<xml_diff>
--- a/Sample Output/Opth0001_dementia.xlsx
+++ b/Sample Output/Opth0001_dementia.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Timepoint 1</t>
   </si>
@@ -28,6 +28,12 @@
     <t>Feature</t>
   </si>
   <si>
+    <t>Total_Brain_Volume</t>
+  </si>
+  <si>
+    <t>Lesions</t>
+  </si>
+  <si>
     <t>Left_Cerebral_Cortex</t>
   </si>
   <si>
@@ -125,9 +131,6 @@
   </si>
   <si>
     <t>CSF</t>
-  </si>
-  <si>
-    <t>Lesions</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -510,13 +513,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>216363.901702</v>
+        <v>702055.389495</v>
       </c>
       <c r="C2">
-        <v>210382.948221</v>
+        <v>692432.848044</v>
       </c>
       <c r="D2">
-        <v>-2.8</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -524,444 +527,444 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>217479.315374</v>
+        <v>20861.282386</v>
       </c>
       <c r="C3">
-        <v>211679.885892</v>
+        <v>20612.32408</v>
       </c>
       <c r="D3">
-        <v>-2.7</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>129820.814226</v>
+        <v>702055.389495</v>
       </c>
       <c r="C4">
-        <v>131305.87288</v>
+        <v>692432.848044</v>
       </c>
       <c r="D4">
-        <v>1.1</v>
+        <v>-1.4</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>138391.358193</v>
+        <v>216363.901702</v>
       </c>
       <c r="C5">
-        <v>139064.141051</v>
+        <v>210382.948221</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>43376.990916</v>
+        <v>217479.315374</v>
       </c>
       <c r="C6">
-        <v>42509.055112</v>
+        <v>211679.885892</v>
       </c>
       <c r="D6">
-        <v>-2</v>
+        <v>-2.7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>42489.206922</v>
+        <v>129820.814226</v>
       </c>
       <c r="C7">
-        <v>41462.946682</v>
+        <v>131305.87288</v>
       </c>
       <c r="D7">
-        <v>-2.4</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>12952.079447</v>
+        <v>138391.358193</v>
       </c>
       <c r="C8">
-        <v>13143.855066</v>
+        <v>139064.141051</v>
       </c>
       <c r="D8">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>12188.86018</v>
+        <v>43376.990916</v>
       </c>
       <c r="C9">
-        <v>12389.316821</v>
+        <v>42509.055112</v>
       </c>
       <c r="D9">
-        <v>1.6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>3384.294242</v>
+        <v>42489.206922</v>
       </c>
       <c r="C10">
-        <v>3320.398542</v>
+        <v>41462.946682</v>
       </c>
       <c r="D10">
-        <v>-1.9</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>3973.598266</v>
+        <v>12952.079447</v>
       </c>
       <c r="C11">
-        <v>3876.511076</v>
+        <v>13143.855066</v>
       </c>
       <c r="D11">
-        <v>-2.4</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
-        <v>1541.30063</v>
+        <v>12188.86018</v>
       </c>
       <c r="C12">
-        <v>1532.384809</v>
+        <v>12389.316821</v>
       </c>
       <c r="D12">
-        <v>-0.6</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>1672.987502</v>
+        <v>3384.294242</v>
       </c>
       <c r="C13">
-        <v>1637.421468</v>
+        <v>3320.398542</v>
       </c>
       <c r="D13">
-        <v>-2.1</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>2882.265225</v>
+        <v>3973.598266</v>
       </c>
       <c r="C14">
-        <v>2877.466901</v>
+        <v>3876.511076</v>
       </c>
       <c r="D14">
-        <v>-0.2</v>
+        <v>-2.4</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>2708.488099</v>
+        <v>1541.30063</v>
       </c>
       <c r="C15">
-        <v>2696.681429</v>
+        <v>1532.384809</v>
       </c>
       <c r="D15">
-        <v>-0.4</v>
+        <v>-0.6</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>4078.4353</v>
+        <v>1672.987502</v>
       </c>
       <c r="C16">
-        <v>4087.333629</v>
+        <v>1637.421468</v>
       </c>
       <c r="D16">
-        <v>0.2</v>
+        <v>-2.1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
-        <v>3950.083621</v>
+        <v>2882.265225</v>
       </c>
       <c r="C17">
-        <v>3961.549178</v>
+        <v>2877.466901</v>
       </c>
       <c r="D17">
-        <v>0.3</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
-        <v>552.470008</v>
+        <v>2708.488099</v>
       </c>
       <c r="C18">
-        <v>537.3571020000001</v>
+        <v>2696.681429</v>
       </c>
       <c r="D18">
-        <v>-2.7</v>
+        <v>-0.4</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
-        <v>543.452117</v>
+        <v>4078.4353</v>
       </c>
       <c r="C19">
-        <v>532.985835</v>
+        <v>4087.333629</v>
       </c>
       <c r="D19">
-        <v>-1.9</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>14719.269037</v>
+        <v>3950.083621</v>
       </c>
       <c r="C20">
-        <v>14541.180806</v>
+        <v>3961.549178</v>
       </c>
       <c r="D20">
-        <v>-1.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>2307.10325</v>
+        <v>552.470008</v>
       </c>
       <c r="C21">
-        <v>2304.277791</v>
+        <v>537.3571020000001</v>
       </c>
       <c r="D21">
-        <v>-0.1</v>
+        <v>-2.7</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
-        <v>2807.284109</v>
+        <v>543.452117</v>
       </c>
       <c r="C22">
-        <v>2705.534508</v>
+        <v>532.985835</v>
       </c>
       <c r="D22">
-        <v>-3.6</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
-        <v>5078.785924</v>
+        <v>14719.269037</v>
       </c>
       <c r="C23">
-        <v>5080.294255</v>
+        <v>14541.180806</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>-1.2</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
-        <v>1904.840295</v>
+        <v>2307.10325</v>
       </c>
       <c r="C24">
-        <v>1929.677608</v>
+        <v>2304.277791</v>
       </c>
       <c r="D24">
-        <v>1.3</v>
+        <v>-0.1</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>2762.606931</v>
+        <v>2807.284109</v>
       </c>
       <c r="C25">
-        <v>2681.386482</v>
+        <v>2705.534508</v>
       </c>
       <c r="D25">
-        <v>-2.9</v>
+        <v>-3.6</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>4548.971697</v>
+        <v>5078.785924</v>
       </c>
       <c r="C26">
-        <v>4540.235741</v>
+        <v>5080.294255</v>
       </c>
       <c r="D26">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
-        <v>29540.644166</v>
+        <v>1904.840295</v>
       </c>
       <c r="C27">
-        <v>30892.433138</v>
+        <v>1929.677608</v>
       </c>
       <c r="D27">
-        <v>4.6</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28">
-        <v>26514.731298</v>
+        <v>2762.606931</v>
       </c>
       <c r="C28">
-        <v>27741.226193</v>
+        <v>2681.386482</v>
       </c>
       <c r="D28">
-        <v>4.6</v>
+        <v>-2.9</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29">
-        <v>858.196462</v>
+        <v>4548.971697</v>
       </c>
       <c r="C29">
-        <v>940.390008</v>
+        <v>4540.235741</v>
       </c>
       <c r="D29">
-        <v>9.6</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>694.158335</v>
+        <v>29540.644166</v>
       </c>
       <c r="C30">
-        <v>774.1007540000001</v>
+        <v>30892.433138</v>
       </c>
       <c r="D30">
-        <v>11.5</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>1993.551358</v>
+        <v>26514.731298</v>
       </c>
       <c r="C31">
-        <v>2052.609872</v>
+        <v>27741.226193</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32">
-        <v>1192.331951</v>
+        <v>858.196462</v>
       </c>
       <c r="C32">
-        <v>1172.213845</v>
+        <v>940.390008</v>
       </c>
       <c r="D32">
-        <v>-1.7</v>
+        <v>9.6</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33">
-        <v>6.896968</v>
+        <v>694.158335</v>
       </c>
       <c r="C33">
-        <v>6.687121</v>
+        <v>774.1007540000001</v>
       </c>
       <c r="D33">
-        <v>-3</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34">
-        <v>389216.034081</v>
+        <v>1993.551358</v>
       </c>
       <c r="C34">
-        <v>400722.91654</v>
+        <v>2052.609872</v>
       </c>
       <c r="D34">
         <v>3</v>
@@ -969,16 +972,44 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>1192.331951</v>
+      </c>
+      <c r="C35">
+        <v>1172.213845</v>
+      </c>
+      <c r="D35">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B35">
-        <v>20861.282386</v>
-      </c>
-      <c r="C35">
-        <v>20612.32408</v>
-      </c>
-      <c r="D35">
-        <v>-1.2</v>
+      <c r="B36">
+        <v>6.896968</v>
+      </c>
+      <c r="C36">
+        <v>6.687121</v>
+      </c>
+      <c r="D36">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>389216.034081</v>
+      </c>
+      <c r="C37">
+        <v>400722.91654</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>